<commit_message>
Handle multi row inline strings
The inline string struct is actually the same
as the shared strings struct, reuse it.

Note that Go version 1.10 is required.

Fixes #462
</commit_message>
<xml_diff>
--- a/test/SharedStrings.xlsx
+++ b/test/SharedStrings.xlsx
@@ -1,60 +1,127 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mh039333/Github/excelize/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB5FB47-8689-6440-97CC-D071A948A8F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="21015" windowHeight="7770"/>
+    <workbookView xWindow="5240" yWindow="4100" windowWidth="21020" windowHeight="7780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
-<file path=xl/SharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Test Weight (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Kgs</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF60759B"/>
+        <bgColor rgb="FF60759B"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF696969"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF696969"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF696969"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF696969"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -63,9 +130,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -73,6 +143,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -119,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -151,9 +229,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,6 +281,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -360,14 +474,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -376,4 +490,22 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7102A20-7A6B-724A-A37A-618412490961}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>